<commit_message>
Added smoke tests to: - Create new Manufacturer/AuthorisedRep - Approve the new account - Search and edit the new Manufacturer/AuthorisedRep
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -433,7 +433,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,6 +574,9 @@
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -582,6 +585,9 @@
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -589,6 +595,9 @@
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed failing tests due to minor changes to manufacturer links etc
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -550,6 +550,9 @@
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -558,6 +561,9 @@
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -565,6 +571,9 @@
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
No need to create users.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7635"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="DeviceSetupLogins" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,12 +617,186 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Trying to add devices to newlyl created users
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7635"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="DeviceSetupLogins" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="InjectSpecificUser" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="33">
   <si>
     <t>username</t>
   </si>
@@ -463,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,91 +491,91 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -584,12 +584,12 @@
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -598,12 +598,12 @@
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
@@ -612,90 +612,132 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -710,7 +752,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +783,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>26</v>
@@ -755,7 +797,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -769,7 +811,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
@@ -783,7 +825,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -797,7 +839,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -811,7 +853,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -992,12 +1034,286 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored the structure of creating devices directly
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -517,7 +517,7 @@
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -531,7 +531,7 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -758,7 +758,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B16"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,10 +786,10 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -800,10 +800,10 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -814,10 +814,10 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -1042,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1072,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -1086,7 +1086,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -1100,7 +1100,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Fixed issue with driver not setting to null
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -517,7 +517,7 @@
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -531,7 +531,7 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -671,7 +671,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
         <v>28</v>
@@ -685,7 +685,7 @@
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -699,7 +699,7 @@
         <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
         <v>28</v>
@@ -1042,7 +1042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
make sure to select newly created manufacturers and authorisedRep
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -757,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Username/password changed from MHRA12345 TO MHRA123456
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="35">
   <si>
     <t>username</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>MHRA12345</t>
+  </si>
+  <si>
+    <t>MHRA123456</t>
   </si>
 </sst>
 </file>
@@ -468,14 +471,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -497,7 +500,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -511,7 +514,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -525,7 +528,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -539,7 +542,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -553,7 +556,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -567,7 +570,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
@@ -1039,7 +1042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Injecting data for users
- Made it more dynamic, so we can inject data for multiple users
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -475,7 +475,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +506,7 @@
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
@@ -520,7 +520,7 @@
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -534,7 +534,7 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Added more test to Manufacturer smoke test - create new manufacturer - add devices - login as business and approve it
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -506,7 +506,7 @@
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
@@ -520,7 +520,7 @@
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -534,7 +534,7 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Username field now required when creating new accounts
Manufacturer_NU
Manufacutrer_AT
AuthorisedRep_NU
AuthorisedRep_AT
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="40">
   <si>
     <t>username</t>
   </si>
@@ -159,6 +159,18 @@
   </si>
   <si>
     <t>MHRA12345A</t>
+  </si>
+  <si>
+    <t>Manufacturer_AT</t>
+  </si>
+  <si>
+    <t>AuthorisedRep_AT</t>
+  </si>
+  <si>
+    <t>Manufacturer_NU</t>
+  </si>
+  <si>
+    <t>AuthorisedRep_NU</t>
   </si>
 </sst>
 </file>
@@ -520,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,35 +602,35 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
@@ -632,169 +644,225 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Smoke tests data creation will no longer work - We need to update password and than create devices - Email is sent with a temporary password
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -163,16 +163,16 @@
     <t>MHRA12345A</t>
   </si>
   <si>
-    <t>Manufacturer_AT</t>
-  </si>
-  <si>
-    <t>AuthorisedRep_AT</t>
-  </si>
-  <si>
-    <t>Manufacturer_NU</t>
-  </si>
-  <si>
-    <t>AuthorisedRep_NU</t>
+    <t>Manufacturer86_AT</t>
+  </si>
+  <si>
+    <t>AuthorisedRep861_AT</t>
+  </si>
+  <si>
+    <t>Manufacturer86_NU</t>
+  </si>
+  <si>
+    <t>AuthorisedRep86_NU</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed some of the failing smoke tests
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -163,16 +163,16 @@
     <t>MHRA12345A</t>
   </si>
   <si>
-    <t>Manufacturer126_AT</t>
-  </si>
-  <si>
-    <t>AuthorisedRep126_AT</t>
-  </si>
-  <si>
-    <t>Manufacturer126_NU</t>
-  </si>
-  <si>
-    <t>AuthorisedRep126_NU</t>
+    <t>Manufacturer196_AT</t>
+  </si>
+  <si>
+    <t>Manufacturer196_NU</t>
+  </si>
+  <si>
+    <t>AuthorisedRep196_NU</t>
+  </si>
+  <si>
+    <t>AuthorisedRep1961_AT</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +590,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>35</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Fixed smoke tests failures due to: - removal of "Remember me" - Introduction of session (no longer can login with same user in multiple browsers)
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -8,10 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="DeviceSetupLogins" sheetId="2" r:id="rId2"/>
-    <sheet name="InjectSpecificUser" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
+    <sheet name="DeviceSetupLogins_REMOVE" sheetId="2" r:id="rId4"/>
+    <sheet name="InjectSpecificUser_REMOVE" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -163,13 +163,13 @@
     <t>MHRA12345A</t>
   </si>
   <si>
+    <t>Manufacturer196_NU</t>
+  </si>
+  <si>
+    <t>AuthorisedRep196_NU</t>
+  </si>
+  <si>
     <t>Manufacturer196_AT</t>
-  </si>
-  <si>
-    <t>Manufacturer196_NU</t>
-  </si>
-  <si>
-    <t>AuthorisedRep196_NU</t>
   </si>
   <si>
     <t>AuthorisedRep1961_AT</t>
@@ -537,7 +537,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +576,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>35</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
@@ -820,6 +820,93 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -1104,12 +1191,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,91 +1476,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Created 4 new users:
Manufacturer371_AT
Manufacturer371_NU
AuthorisedRep371_AT
AuthorisedRep371_NU
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -163,16 +163,16 @@
     <t>MHRA12345A</t>
   </si>
   <si>
-    <t>Manufacturer196_NU</t>
-  </si>
-  <si>
-    <t>AuthorisedRep196_NU</t>
-  </si>
-  <si>
-    <t>Manufacturer196_AT</t>
-  </si>
-  <si>
-    <t>AuthorisedRep1961_AT</t>
+    <t>Manufacturer371_AT</t>
+  </si>
+  <si>
+    <t>AuthorisedRep371_AT</t>
+  </si>
+  <si>
+    <t>Manufacturer371_NU</t>
+  </si>
+  <si>
+    <t>AuthorisedRep371_NU</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +568,7 @@
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
@@ -576,13 +576,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -590,13 +590,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
@@ -610,7 +610,7 @@
         <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -618,13 +618,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
@@ -632,13 +632,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
We should be able to control the max number of devices we add during device registration, so that it doesn't take very long.
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -537,7 +537,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +565,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Changed payments to : BACS as WorldPay requires too many changees
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -8,10 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
-    <sheet name="DeviceSetupLogins_REMOVE" sheetId="2" r:id="rId4"/>
-    <sheet name="InjectSpecificUser_REMOVE" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId2"/>
+    <sheet name="DeviceSetupLogins_REMOVE" sheetId="2" r:id="rId3"/>
+    <sheet name="InjectSpecificUser_REMOVE" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -53,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="40">
   <si>
     <t>username</t>
   </si>
@@ -157,9 +156,6 @@
     <t>MHRA12345</t>
   </si>
   <si>
-    <t>MHRA123456</t>
-  </si>
-  <si>
     <t>MHRA12345A</t>
   </si>
   <si>
@@ -173,6 +169,9 @@
   </si>
   <si>
     <t>AuthorisedRep127H9_AT</t>
+  </si>
+  <si>
+    <t>MHRA12345B</t>
   </si>
 </sst>
 </file>
@@ -537,7 +536,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +564,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -576,10 +575,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -590,10 +589,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -607,7 +606,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -618,10 +617,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -632,10 +631,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
@@ -775,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
@@ -789,7 +788,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -803,7 +802,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -820,81 +819,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -906,7 +830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -1191,7 +1115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>

</xml_diff>

<commit_message>
Smoke tests failing due to incorrect login details
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -148,13 +148,13 @@
     <t>AuthorisedRep177H10_AT</t>
   </si>
   <si>
-    <t>Manufacturer177H7_NU</t>
-  </si>
-  <si>
-    <t>AuthorisedRep177H7_NU</t>
-  </si>
-  <si>
     <t>MHRA12345D</t>
+  </si>
+  <si>
+    <t>Manufacturer267H7_NU</t>
+  </si>
+  <si>
+    <t>AuthorisedRep267H8_NU</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +589,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
@@ -600,7 +600,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>29</v>
@@ -614,7 +614,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Introduced a new page to accept Terms and conditions
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -142,19 +142,19 @@
     <t>MHRA12345A</t>
   </si>
   <si>
-    <t>Manufacturer177H9_AT</t>
-  </si>
-  <si>
-    <t>AuthorisedRep177H10_AT</t>
-  </si>
-  <si>
     <t>MHRA12345D</t>
   </si>
   <si>
-    <t>Manufacturer267H7_NU</t>
-  </si>
-  <si>
-    <t>AuthorisedRep267H8_NU</t>
+    <t>Manufacturer277H12_AT</t>
+  </si>
+  <si>
+    <t>AuthorisedRep277H12_AT</t>
+  </si>
+  <si>
+    <t>Manufacturer277H12_NU</t>
+  </si>
+  <si>
+    <t>AuthorisedRep277H12_NU</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>29</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>29</v>
@@ -589,7 +589,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Timeout changed from default to normal
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
   <si>
     <t>username</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t>MHRA12345F</t>
+  </si>
+  <si>
+    <t>priya.giri</t>
+  </si>
+  <si>
+    <t>password3</t>
+  </si>
+  <si>
+    <t>PG</t>
   </si>
 </sst>
 </file>
@@ -516,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +601,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -606,7 +615,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -620,7 +629,7 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -792,6 +801,48 @@
       </c>
       <c r="D19" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Properties file will control which users to run smoke tests for
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
   <si>
     <t>username</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>PG</t>
+  </si>
+  <si>
+    <t>Manufacturer78H14_PG</t>
+  </si>
+  <si>
+    <t>AuthorisedRep78H14_PG</t>
   </si>
 </sst>
 </file>
@@ -528,7 +534,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +607,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -615,7 +621,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -629,7 +635,7 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -811,7 +817,7 @@
         <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
         <v>37</v>
@@ -819,13 +825,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
         <v>37</v>
@@ -833,13 +839,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Minor issues with creating new accounts and organisations
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -157,9 +157,6 @@
     <t>MHRA12345F</t>
   </si>
   <si>
-    <t>priya.giri</t>
-  </si>
-  <si>
     <t>password3</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>AuthorisedRep78H14_PG</t>
+  </si>
+  <si>
+    <t>Priya.Giri.Business</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,21 +811,21 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
         <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>29</v>
@@ -834,12 +834,12 @@
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>29</v>
@@ -848,7 +848,7 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
We should be able to run smoke tests in Preprod and Test
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId2"/>
+    <sheet name="PreProdEnv" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -49,8 +49,43 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>TPD_Auto</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>TPD_Auto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+IGNORE FOR SMOKE TESTS
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="40">
   <si>
     <t>username</t>
   </si>
@@ -533,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,13 +894,330 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added manufacturer account details for priya
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="14730" windowHeight="7290"/>
   </bookViews>
   <sheets>
     <sheet name="TestEnv" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="44">
   <si>
     <t>username</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>MHRA12345A@</t>
+  </si>
+  <si>
+    <t>Manufacturer1681H8_PG</t>
+  </si>
+  <si>
+    <t>AuthorisedRep1681H9_PG</t>
   </si>
 </sst>
 </file>
@@ -574,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +872,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>29</v>
@@ -880,7 +886,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>29</v>
@@ -903,7 +909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>